<commit_message>
initial plots for NC
</commit_message>
<xml_diff>
--- a/data/North_Carolina/aptest2020_(2018_20)northcarolina.xlsx
+++ b/data/North_Carolina/aptest2020_(2018_20)northcarolina.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4E1B15A24CE88334/Documents/APdata/North_Carolina/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amahapatra\Documents\data_sc\git_clone_AP\AP-Outcomes-to-University-Metrics\data\North_Carolina\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3A52230C-0717-41C1-8E76-DE034A33A540}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16F1A9B4-F4A0-490E-99E8-4D8EAFC72BEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="24" yWindow="384" windowWidth="23016" windowHeight="13656" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2019-2020" sheetId="1" r:id="rId1"/>
@@ -3029,6 +3029,18 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -3049,18 +3061,6 @@
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -3386,7 +3386,7 @@
   <dimension ref="A1:AA665"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="B528" sqref="B528"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3401,42 +3401,42 @@
       <c r="A1" s="2"/>
       <c r="B1" s="3"/>
       <c r="C1" s="4"/>
-      <c r="D1" s="53">
+      <c r="D1" s="57">
         <v>2018</v>
       </c>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54"/>
-      <c r="I1" s="54"/>
-      <c r="J1" s="55"/>
+      <c r="E1" s="58"/>
+      <c r="F1" s="58"/>
+      <c r="G1" s="58"/>
+      <c r="H1" s="58"/>
+      <c r="I1" s="58"/>
+      <c r="J1" s="59"/>
       <c r="K1" s="5"/>
-      <c r="L1" s="53">
+      <c r="L1" s="57">
         <v>2019</v>
       </c>
-      <c r="M1" s="54"/>
-      <c r="N1" s="54"/>
-      <c r="O1" s="54"/>
-      <c r="P1" s="54"/>
-      <c r="Q1" s="54"/>
-      <c r="R1" s="55"/>
+      <c r="M1" s="58"/>
+      <c r="N1" s="58"/>
+      <c r="O1" s="58"/>
+      <c r="P1" s="58"/>
+      <c r="Q1" s="58"/>
+      <c r="R1" s="59"/>
       <c r="S1" s="5"/>
-      <c r="T1" s="53">
+      <c r="T1" s="57">
         <v>2020</v>
       </c>
-      <c r="U1" s="54"/>
-      <c r="V1" s="54"/>
-      <c r="W1" s="54"/>
-      <c r="X1" s="54"/>
-      <c r="Y1" s="54"/>
-      <c r="Z1" s="55"/>
+      <c r="U1" s="58"/>
+      <c r="V1" s="58"/>
+      <c r="W1" s="58"/>
+      <c r="X1" s="58"/>
+      <c r="Y1" s="58"/>
+      <c r="Z1" s="59"/>
     </row>
     <row r="2" spans="1:26" s="6" customFormat="1" ht="79.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
-      <c r="B2" s="56" t="s">
+      <c r="B2" s="60" t="s">
         <v>666</v>
       </c>
-      <c r="C2" s="57"/>
+      <c r="C2" s="61"/>
       <c r="D2" s="7" t="s">
         <v>667</v>
       </c>
@@ -47975,10 +47975,10 @@
       <c r="A608" s="42" t="s">
         <v>597</v>
       </c>
-      <c r="B608" s="51" t="s">
+      <c r="B608" s="55" t="s">
         <v>677</v>
       </c>
-      <c r="C608" s="52"/>
+      <c r="C608" s="56"/>
       <c r="D608" s="14">
         <v>6</v>
       </c>
@@ -48410,10 +48410,10 @@
       <c r="A614" s="42" t="s">
         <v>605</v>
       </c>
-      <c r="B614" s="51" t="s">
+      <c r="B614" s="55" t="s">
         <v>681</v>
       </c>
-      <c r="C614" s="52"/>
+      <c r="C614" s="56"/>
       <c r="D614" s="14">
         <v>24</v>
       </c>
@@ -48546,10 +48546,10 @@
       <c r="A616" s="42" t="s">
         <v>608</v>
       </c>
-      <c r="B616" s="51" t="s">
+      <c r="B616" s="55" t="s">
         <v>682</v>
       </c>
-      <c r="C616" s="52"/>
+      <c r="C616" s="56"/>
       <c r="D616" s="14"/>
       <c r="E616" s="24"/>
       <c r="F616" s="14"/>
@@ -48606,10 +48606,10 @@
       <c r="A617" s="42" t="s">
         <v>609</v>
       </c>
-      <c r="B617" s="51" t="s">
+      <c r="B617" s="55" t="s">
         <v>683</v>
       </c>
-      <c r="C617" s="52" t="s">
+      <c r="C617" s="56" t="s">
         <v>0</v>
       </c>
       <c r="D617" s="14" t="s">
@@ -48741,10 +48741,10 @@
       <c r="A619" s="42" t="s">
         <v>611</v>
       </c>
-      <c r="B619" s="52" t="s">
+      <c r="B619" s="56" t="s">
         <v>685</v>
       </c>
-      <c r="C619" s="52"/>
+      <c r="C619" s="56"/>
       <c r="D619" s="14">
         <v>18</v>
       </c>
@@ -49302,10 +49302,10 @@
       <c r="A627" s="42" t="s">
         <v>622</v>
       </c>
-      <c r="B627" s="52" t="s">
+      <c r="B627" s="56" t="s">
         <v>690</v>
       </c>
-      <c r="C627" s="52"/>
+      <c r="C627" s="56"/>
       <c r="D627" s="14">
         <v>22</v>
       </c>
@@ -49378,10 +49378,10 @@
       <c r="A628" s="42" t="s">
         <v>623</v>
       </c>
-      <c r="B628" s="59" t="s">
+      <c r="B628" s="51" t="s">
         <v>691</v>
       </c>
-      <c r="C628" s="58"/>
+      <c r="C628" s="52"/>
       <c r="D628" s="14">
         <v>89</v>
       </c>
@@ -49530,10 +49530,10 @@
       <c r="A630" s="42" t="s">
         <v>625</v>
       </c>
-      <c r="B630" s="58" t="s">
+      <c r="B630" s="52" t="s">
         <v>693</v>
       </c>
-      <c r="C630" s="58"/>
+      <c r="C630" s="52"/>
       <c r="D630" s="14">
         <v>66</v>
       </c>
@@ -49971,10 +49971,10 @@
       <c r="A636" s="42" t="s">
         <v>632</v>
       </c>
-      <c r="B636" s="51" t="s">
+      <c r="B636" s="55" t="s">
         <v>697</v>
       </c>
-      <c r="C636" s="52"/>
+      <c r="C636" s="56"/>
       <c r="D636" s="14">
         <v>15</v>
       </c>
@@ -50345,10 +50345,10 @@
       <c r="A641" s="42" t="s">
         <v>637</v>
       </c>
-      <c r="B641" s="58" t="s">
+      <c r="B641" s="52" t="s">
         <v>701</v>
       </c>
-      <c r="C641" s="58" t="s">
+      <c r="C641" s="52" t="s">
         <v>0</v>
       </c>
       <c r="D641" s="14">
@@ -50884,10 +50884,10 @@
       <c r="A649" s="42" t="s">
         <v>646</v>
       </c>
-      <c r="B649" s="59" t="s">
+      <c r="B649" s="51" t="s">
         <v>707</v>
       </c>
-      <c r="C649" s="58"/>
+      <c r="C649" s="52"/>
       <c r="D649" s="14">
         <v>75</v>
       </c>
@@ -50960,10 +50960,10 @@
       <c r="A650" s="42" t="s">
         <v>647</v>
       </c>
-      <c r="B650" s="59" t="s">
+      <c r="B650" s="51" t="s">
         <v>708</v>
       </c>
-      <c r="C650" s="58" t="s">
+      <c r="C650" s="52" t="s">
         <v>0</v>
       </c>
       <c r="D650" s="14" t="s">
@@ -51216,10 +51216,10 @@
       <c r="A654" s="42" t="s">
         <v>652</v>
       </c>
-      <c r="B654" s="58" t="s">
+      <c r="B654" s="52" t="s">
         <v>711</v>
       </c>
-      <c r="C654" s="58"/>
+      <c r="C654" s="52"/>
       <c r="D654" s="14">
         <v>13</v>
       </c>
@@ -51368,10 +51368,10 @@
       <c r="A656" s="42" t="s">
         <v>654</v>
       </c>
-      <c r="B656" s="59" t="s">
+      <c r="B656" s="51" t="s">
         <v>713</v>
       </c>
-      <c r="C656" s="58"/>
+      <c r="C656" s="52"/>
       <c r="D656" s="14">
         <v>29</v>
       </c>
@@ -51444,10 +51444,10 @@
       <c r="A657" s="42" t="s">
         <v>655</v>
       </c>
-      <c r="B657" s="59" t="s">
+      <c r="B657" s="51" t="s">
         <v>714</v>
       </c>
-      <c r="C657" s="58"/>
+      <c r="C657" s="52"/>
       <c r="D657" s="14">
         <v>101</v>
       </c>
@@ -51969,10 +51969,10 @@
       <c r="A664" s="42" t="s">
         <v>663</v>
       </c>
-      <c r="B664" s="59" t="s">
+      <c r="B664" s="51" t="s">
         <v>719</v>
       </c>
-      <c r="C664" s="58"/>
+      <c r="C664" s="52"/>
       <c r="D664" s="14">
         <v>68</v>
       </c>
@@ -52045,10 +52045,10 @@
       <c r="A665" s="23" t="s">
         <v>664</v>
       </c>
-      <c r="B665" s="60" t="s">
+      <c r="B665" s="53" t="s">
         <v>720</v>
       </c>
-      <c r="C665" s="61" t="s">
+      <c r="C665" s="54" t="s">
         <v>0</v>
       </c>
       <c r="D665" s="30">
@@ -52122,27 +52122,27 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="B656:C656"/>
-    <mergeCell ref="B657:C657"/>
-    <mergeCell ref="B664:C664"/>
-    <mergeCell ref="B665:C665"/>
-    <mergeCell ref="B654:C654"/>
-    <mergeCell ref="B616:C616"/>
-    <mergeCell ref="B617:C617"/>
-    <mergeCell ref="B619:C619"/>
-    <mergeCell ref="B627:C627"/>
-    <mergeCell ref="B628:C628"/>
-    <mergeCell ref="B630:C630"/>
-    <mergeCell ref="B636:C636"/>
-    <mergeCell ref="B641:C641"/>
-    <mergeCell ref="B649:C649"/>
-    <mergeCell ref="B650:C650"/>
     <mergeCell ref="B614:C614"/>
     <mergeCell ref="D1:J1"/>
     <mergeCell ref="L1:R1"/>
     <mergeCell ref="T1:Z1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B608:C608"/>
+    <mergeCell ref="B630:C630"/>
+    <mergeCell ref="B636:C636"/>
+    <mergeCell ref="B641:C641"/>
+    <mergeCell ref="B649:C649"/>
+    <mergeCell ref="B650:C650"/>
+    <mergeCell ref="B616:C616"/>
+    <mergeCell ref="B617:C617"/>
+    <mergeCell ref="B619:C619"/>
+    <mergeCell ref="B627:C627"/>
+    <mergeCell ref="B628:C628"/>
+    <mergeCell ref="B656:C656"/>
+    <mergeCell ref="B657:C657"/>
+    <mergeCell ref="B664:C664"/>
+    <mergeCell ref="B665:C665"/>
+    <mergeCell ref="B654:C654"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
@@ -52150,6 +52150,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A2561A5AE02506468B410A1B121BCE68" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="6bdb0360f990a7a604b86168db7f094d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns3="634404f4-ad08-4a1f-b211-23d910c32ca2" xmlns:ns4="7d67d2f0-c194-45cf-acc0-a941baafef4d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5ca79945bb2efaf1ec89eea3ec7ada23" ns1:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -52377,15 +52386,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -52396,6 +52396,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AD67EE06-5822-44D7-A8A7-312D6E3C0C6A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4512BF3E-C7DF-4620-85D8-DFF6325A33C0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -52415,14 +52423,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AD67EE06-5822-44D7-A8A7-312D6E3C0C6A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AA09B2D8-C213-42F2-8ABB-B2B18A6ABD96}">
   <ds:schemaRefs>

</xml_diff>